<commit_message>
Changes to Excel quiz 4 to better format a table and chart.
</commit_message>
<xml_diff>
--- a/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 4.xlsx
+++ b/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggobl\Documents\Portfolio\Excel\INFS 768 - Predictive Analytics\Quizzes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7309AEEA-A42B-4E61-B9E7-9AE0822DBF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09E3567-880E-4094-9AED-DCEC5831E4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{844688FB-E543-4218-B9C2-F57D99FDB6AB}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Original Points</t>
   </si>
@@ -178,11 +178,14 @@
   <si>
     <t>Distance between 2 lines formula:</t>
   </si>
+  <si>
+    <t>Classes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,16 +229,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{7DFDA3E8-3338-4C67-82EC-BA17A6B5F4C4}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -270,7 +293,7 @@
           <c:yMode val="edge"/>
           <c:x val="7.2886482939632541E-2"/>
           <c:y val="4.1666666666666664E-2"/>
-          <c:w val="0.39462751531058615"/>
+          <c:w val="0.56920478025353216"/>
           <c:h val="0.8416746864975212"/>
         </c:manualLayout>
       </c:layout>
@@ -375,7 +398,7 @@
             <c:numRef>
               <c:f>Sheet1!$F$22:$F$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
@@ -390,7 +413,7 @@
             <c:numRef>
               <c:f>Sheet1!$G$22:$G$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -506,7 +529,7 @@
             <c:numRef>
               <c:f>Sheet1!$F$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
@@ -518,7 +541,7 @@
             <c:numRef>
               <c:f>Sheet1!$G$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
@@ -1226,7 +1249,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1288,7 +1311,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1340,6 +1363,18 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
         <c:idx val="8"/>
         <c:delete val="1"/>
       </c:legendEntry>
@@ -1355,6 +1390,16 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7007730109841015"/>
+          <c:y val="0.30931576261300675"/>
+          <c:w val="0.14374417395861522"/>
+          <c:h val="0.39062773403324585"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2049,11 +2094,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{52632F28-5827-4CC9-8C85-BE544D43A770}" name="Table4" displayName="Table4" ref="F21:G24" totalsRowShown="0">
-  <autoFilter ref="F21:G24" xr:uid="{52632F28-5827-4CC9-8C85-BE544D43A770}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4ACA855A-30B7-43E3-8C1D-25457D50649A}" name="x"/>
-    <tableColumn id="2" xr3:uid="{C4E0E110-B7CF-4BA1-944A-44AB555258B7}" name="y"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{52632F28-5827-4CC9-8C85-BE544D43A770}" name="Table4" displayName="Table4" ref="F21:H24" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="F21:H24" xr:uid="{52632F28-5827-4CC9-8C85-BE544D43A770}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4ACA855A-30B7-43E3-8C1D-25457D50649A}" name="x" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C4E0E110-B7CF-4BA1-944A-44AB555258B7}" name="y" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00ADC5FF-573B-4EA1-9F66-D8204189B11F}" name="Classes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2359,7 +2405,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2477,7 +2523,7 @@
         <v>-1.0000009999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2494,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2507,14 +2553,18 @@
       <c r="D21" t="s">
         <v>22</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="H21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2530,17 +2580,17 @@
         <f>4-$A22/2</f>
         <v>3.5</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="4">
         <v>2</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="4">
         <v>0</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2556,17 +2606,17 @@
         <f t="shared" ref="D23:D27" si="2">4-$A23/2</f>
         <v>3</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="4">
         <v>1</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="4">
         <v>1</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2582,17 +2632,17 @@
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="4">
         <v>2</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="4">
         <v>3</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2609,7 +2659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2626,7 +2676,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2646,7 +2696,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2659,7 +2709,7 @@
         <v>2.2360679774997898</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E31">
         <f>(3-1)/(2-1)</f>
         <v>2</v>

</xml_diff>